<commit_message>
Daily notes and Feedback points added
Also updated the refinement documents
</commit_message>
<xml_diff>
--- a/Project documentation/3. Realization/Issue estimates.xlsx
+++ b/Project documentation/3. Realization/Issue estimates.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rymga\Desktop\Semester 8\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rymga\Desktop\Semester 8\S8-GI-Drieam\Project documentation\3. Realization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E300B21-8CA4-4E46-B6C3-FB367487E07B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBB0C2E0-C557-4D46-85FE-CE2F4CFB257F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5580" yWindow="-17388" windowWidth="30936" windowHeight="16776" xr2:uid="{1501C23A-469F-491C-9AA1-0DB21E281099}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1501C23A-469F-491C-9AA1-0DB21E281099}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -183,12 +183,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -520,12 +520,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -537,7 +537,7 @@
       <c r="C2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="9" t="s">
         <v>11</v>
       </c>
     </row>
@@ -551,7 +551,7 @@
       <c r="C3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="9">
         <v>9</v>
       </c>
     </row>
@@ -565,7 +565,7 @@
       <c r="C4" s="7">
         <v>1</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="9" t="s">
         <v>12</v>
       </c>
     </row>
@@ -579,7 +579,7 @@
       <c r="C5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="10" t="s">
         <v>14</v>
       </c>
     </row>
@@ -593,7 +593,7 @@
       <c r="C6" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="9" t="s">
         <v>13</v>
       </c>
     </row>
@@ -607,7 +607,7 @@
       <c r="C7" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="10"/>
+      <c r="D7" s="9"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
@@ -619,7 +619,7 @@
       <c r="C8" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="10"/>
+      <c r="D8" s="9"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>

</xml_diff>

<commit_message>
Mid-term evaluation document from mentors
</commit_message>
<xml_diff>
--- a/Project documentation/3. Realization/Issue estimates.xlsx
+++ b/Project documentation/3. Realization/Issue estimates.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rymga\Desktop\Semester 8\S8-GI-Drieam\Project documentation\3. Realization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBB0C2E0-C557-4D46-85FE-CE2F4CFB257F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4CD756E-F6E9-4926-A061-2F13DA808D3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1501C23A-469F-491C-9AA1-0DB21E281099}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="16">
   <si>
     <t>Description</t>
   </si>
@@ -81,13 +81,16 @@
   </si>
   <si>
     <t>3.5</t>
+  </si>
+  <si>
+    <t>Sprint 2023.04.1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -106,6 +109,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -157,11 +168,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -190,8 +202,19 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Explanatory Text" xfId="2" builtinId="53"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -505,18 +528,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{164F14AA-CFE8-4BA4-89BA-FFC874ABC001}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="8.33203125" style="5" customWidth="1"/>
     <col min="2" max="2" width="43.109375" customWidth="1"/>
-    <col min="3" max="3" width="15.88671875" style="8" customWidth="1"/>
-    <col min="4" max="4" width="19.5546875" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" style="8" customWidth="1"/>
+    <col min="4" max="4" width="17.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -579,8 +602,8 @@
       <c r="C5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="10" t="s">
-        <v>14</v>
+      <c r="D5" s="10">
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -607,7 +630,9 @@
       <c r="C7" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="9"/>
+      <c r="D7" s="10" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
@@ -619,12 +644,18 @@
       <c r="C8" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="9"/>
+      <c r="D8" s="1"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="2"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="7"/>
+      <c r="A9" s="12">
+        <v>2862</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>3</v>
+      </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -634,14 +665,87 @@
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="2"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="1"/>
+      <c r="A11" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>2862</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="2"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="2"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="2"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="2"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="9"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="2"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="2"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A11:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Research and wireframe progress
</commit_message>
<xml_diff>
--- a/Project documentation/3. Realization/Issue estimates.xlsx
+++ b/Project documentation/3. Realization/Issue estimates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rymga\Desktop\Semester 8\S8-GI-Drieam\Project documentation\3. Realization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2AAEE1F-E4B6-468B-B589-5F819C110056}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22402F43-3DC6-4F79-8DAB-DE48A6AFB66C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1501C23A-469F-491C-9AA1-0DB21E281099}"/>
+    <workbookView xWindow="10512" yWindow="-15792" windowWidth="17280" windowHeight="14496" xr2:uid="{1501C23A-469F-491C-9AA1-0DB21E281099}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="24">
   <si>
     <t>Description</t>
   </si>
@@ -90,6 +90,24 @@
   </si>
   <si>
     <t>Allow filtering</t>
+  </si>
+  <si>
+    <t>Sprint 2023.04.0 Bristol</t>
+  </si>
+  <si>
+    <t>Sprint 2023.04.0 C****</t>
+  </si>
+  <si>
+    <t>Sprint 2023.04.0 D****</t>
+  </si>
+  <si>
+    <t>Allow filtering on Evidence Type</t>
+  </si>
+  <si>
+    <t>Add Goals to My Evidence Table</t>
+  </si>
+  <si>
+    <t>Rename "Delete" to "Move to trash bin"</t>
   </si>
 </sst>
 </file>
@@ -534,10 +552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{164F14AA-CFE8-4BA4-89BA-FFC874ABC001}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -721,13 +739,13 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="2">
+      <c r="A15" s="11">
         <v>2864</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="13">
         <v>2</v>
       </c>
       <c r="D15" s="9">
@@ -764,14 +782,292 @@
       <c r="B19" s="1"/>
       <c r="C19" s="7"/>
       <c r="D19" s="9">
-        <f>SUM(C13:C15)</f>
-        <v>3</v>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="2"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="15"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="2">
+        <v>2864</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="7">
+        <v>2</v>
+      </c>
+      <c r="D23" s="9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="2">
+        <v>3223</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="2">
+        <v>3227</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" s="7">
+        <v>2</v>
+      </c>
+      <c r="D25" s="9">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="2"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="2"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="10">
+        <f>SUM(C23:C25)</f>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="2"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="2"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="9">
+        <f>SUM(C23:C25)</f>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B31" s="15"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="2">
+        <v>2862</v>
+      </c>
+      <c r="B33" s="1"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="2">
+        <v>2861</v>
+      </c>
+      <c r="B34" s="1"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="2">
+        <v>2864</v>
+      </c>
+      <c r="B35" s="1"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="2"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="2"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="10">
+        <f>SUM(C33:C35)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="2"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="2"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="9">
+        <f>SUM(C33:C35)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B41" s="15"/>
+      <c r="C41" s="15"/>
+      <c r="D41" s="15"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="2">
+        <v>2862</v>
+      </c>
+      <c r="B43" s="1"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="2">
+        <v>2861</v>
+      </c>
+      <c r="B44" s="1"/>
+      <c r="C44" s="7"/>
+      <c r="D44" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="2">
+        <v>2864</v>
+      </c>
+      <c r="B45" s="1"/>
+      <c r="C45" s="7"/>
+      <c r="D45" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="2"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="7"/>
+      <c r="D46" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="2"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="10">
+        <f>SUM(C43:C45)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" s="2"/>
+      <c r="B48" s="1"/>
+      <c r="C48" s="7"/>
+      <c r="D48" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" s="2"/>
+      <c r="B49" s="1"/>
+      <c r="C49" s="7"/>
+      <c r="D49" s="9">
+        <f>SUM(C43:C45)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="5">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A11:D11"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="A31:D31"/>
+    <mergeCell ref="A41:D41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Research documents and design V8
</commit_message>
<xml_diff>
--- a/Project documentation/3. Realization/Issue estimates.xlsx
+++ b/Project documentation/3. Realization/Issue estimates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rymga\Desktop\Semester 8\S8-GI-Drieam\Project documentation\3. Realization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22402F43-3DC6-4F79-8DAB-DE48A6AFB66C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B3F163E-5A3D-490C-BDB4-9AD288C7D4ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10512" yWindow="-15792" windowWidth="17280" windowHeight="14496" xr2:uid="{1501C23A-469F-491C-9AA1-0DB21E281099}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1501C23A-469F-491C-9AA1-0DB21E281099}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="30">
   <si>
     <t>Description</t>
   </si>
@@ -95,9 +95,6 @@
     <t>Sprint 2023.04.0 Bristol</t>
   </si>
   <si>
-    <t>Sprint 2023.04.0 C****</t>
-  </si>
-  <si>
     <t>Sprint 2023.04.0 D****</t>
   </si>
   <si>
@@ -108,13 +105,34 @@
   </si>
   <si>
     <t>Rename "Delete" to "Move to trash bin"</t>
+  </si>
+  <si>
+    <t>Sprint 2023.04.0 Cadiz</t>
+  </si>
+  <si>
+    <t>Add tooltip on delete option</t>
+  </si>
+  <si>
+    <t>Allow users to remove evidence from Collections</t>
+  </si>
+  <si>
+    <t>*once done with the "Convert My Evidence list to a table" epic move it all to testing and ask Elise to test!!!!!</t>
+  </si>
+  <si>
+    <t>asign the epic to elise when doing so</t>
+  </si>
+  <si>
+    <t>Disable delete for evidence linked to goals</t>
+  </si>
+  <si>
+    <t>Add icons to the actions options in My Evidence page</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -141,6 +159,13 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -197,7 +222,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -236,6 +261,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Explanatory Text" xfId="2" builtinId="53"/>
@@ -552,16 +578,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{164F14AA-CFE8-4BA4-89BA-FFC874ABC001}">
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.33203125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="43.109375" customWidth="1"/>
+    <col min="2" max="2" width="44.77734375" customWidth="1"/>
     <col min="3" max="3" width="12.5546875" style="8" customWidth="1"/>
     <col min="4" max="4" width="17.109375" customWidth="1"/>
   </cols>
@@ -818,7 +844,7 @@
         <v>2864</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C23" s="7">
         <v>2</v>
@@ -832,7 +858,7 @@
         <v>3223</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C24" s="7">
         <v>0.5</v>
@@ -846,7 +872,7 @@
         <v>3227</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C25" s="7">
         <v>2</v>
@@ -891,7 +917,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="15" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B31" s="15"/>
       <c r="C31" s="15"/>
@@ -911,54 +937,78 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
-        <v>2862</v>
-      </c>
-      <c r="B33" s="1"/>
-      <c r="C33" s="7"/>
+        <v>3225</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C33" s="7">
+        <v>0.5</v>
+      </c>
       <c r="D33" s="9">
         <v>8</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E33" s="16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
-        <v>2861</v>
-      </c>
-      <c r="B34" s="1"/>
-      <c r="C34" s="7"/>
+        <v>3230</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C34" s="7">
+        <v>1</v>
+      </c>
       <c r="D34" s="9" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E34" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
-        <v>2864</v>
-      </c>
-      <c r="B35" s="1"/>
-      <c r="C35" s="7"/>
+        <v>3229</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C35" s="7">
+        <v>0.5</v>
+      </c>
       <c r="D35" s="9">
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="2"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="7"/>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="2">
+        <v>3226</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C36" s="7">
+        <v>0.5</v>
+      </c>
       <c r="D36" s="9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="2"/>
       <c r="B37" s="1"/>
       <c r="C37" s="7"/>
       <c r="D37" s="10">
         <f>SUM(C33:C35)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="2"/>
       <c r="B38" s="1"/>
       <c r="C38" s="7"/>
@@ -966,24 +1016,24 @@
         <v>13</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="2"/>
       <c r="B39" s="1"/>
       <c r="C39" s="7"/>
       <c r="D39" s="9">
-        <f>SUM(C33:C35)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+        <f>SUM(C33:C37)</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B41" s="15"/>
       <c r="C41" s="15"/>
       <c r="D41" s="15"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>5</v>
       </c>
@@ -997,7 +1047,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <v>2862</v>
       </c>
@@ -1007,7 +1057,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>2861</v>
       </c>
@@ -1017,7 +1067,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>2864</v>
       </c>
@@ -1027,7 +1077,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="2"/>
       <c r="B46" s="1"/>
       <c r="C46" s="7"/>
@@ -1035,7 +1085,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="2"/>
       <c r="B47" s="1"/>
       <c r="C47" s="7"/>
@@ -1044,7 +1094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="2"/>
       <c r="B48" s="1"/>
       <c r="C48" s="7"/>

</xml_diff>

<commit_message>
TICT and Research progress
</commit_message>
<xml_diff>
--- a/Project documentation/3. Realization/Issue estimates.xlsx
+++ b/Project documentation/3. Realization/Issue estimates.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rymga\Desktop\Semester 8\S8-GI-Drieam\Project documentation\3. Realization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B3F163E-5A3D-490C-BDB4-9AD288C7D4ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CF040C9-BDEB-409E-88FE-06D2D0F185C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1501C23A-469F-491C-9AA1-0DB21E281099}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="34">
   <si>
     <t>Description</t>
   </si>
@@ -95,9 +95,6 @@
     <t>Sprint 2023.04.0 Bristol</t>
   </si>
   <si>
-    <t>Sprint 2023.04.0 D****</t>
-  </si>
-  <si>
     <t>Allow filtering on Evidence Type</t>
   </si>
   <si>
@@ -126,6 +123,21 @@
   </si>
   <si>
     <t>Add icons to the actions options in My Evidence page</t>
+  </si>
+  <si>
+    <t>Allow filtering by collections</t>
+  </si>
+  <si>
+    <t>Sprint 2023.04.0 Donetsk</t>
+  </si>
+  <si>
+    <t>Allow filtering on feedback status</t>
+  </si>
+  <si>
+    <t>Allow filtering on goals</t>
+  </si>
+  <si>
+    <t>Allow filtering by creation date</t>
   </si>
 </sst>
 </file>
@@ -255,13 +267,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Explanatory Text" xfId="2" builtinId="53"/>
@@ -580,8 +592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{164F14AA-CFE8-4BA4-89BA-FFC874ABC001}">
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -593,12 +605,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -715,12 +727,12 @@
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
@@ -818,12 +830,12 @@
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="15" t="s">
+      <c r="A21" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="15"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
@@ -844,7 +856,7 @@
         <v>2864</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C23" s="7">
         <v>2</v>
@@ -858,7 +870,7 @@
         <v>3223</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C24" s="7">
         <v>0.5</v>
@@ -872,7 +884,7 @@
         <v>3227</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C25" s="7">
         <v>2</v>
@@ -916,12 +928,12 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B31" s="15"/>
-      <c r="C31" s="15"/>
-      <c r="D31" s="15"/>
+      <c r="A31" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B31" s="16"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="16"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
@@ -942,16 +954,16 @@
         <v>3225</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C33" s="7">
         <v>0.5</v>
       </c>
       <c r="D33" s="9">
-        <v>8</v>
-      </c>
-      <c r="E33" s="16" t="s">
-        <v>26</v>
+        <v>7</v>
+      </c>
+      <c r="E33" s="14" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
@@ -959,7 +971,7 @@
         <v>3230</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C34" s="7">
         <v>1</v>
@@ -968,7 +980,7 @@
         <v>15</v>
       </c>
       <c r="E34" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
@@ -976,7 +988,7 @@
         <v>3229</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C35" s="7">
         <v>0.5</v>
@@ -990,7 +1002,7 @@
         <v>3226</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C36" s="7">
         <v>0.5</v>
@@ -1000,12 +1012,18 @@
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" s="2"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="7"/>
+      <c r="A37" s="2">
+        <v>3222</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C37" s="7">
+        <v>1</v>
+      </c>
       <c r="D37" s="10">
-        <f>SUM(C33:C35)</f>
-        <v>2</v>
+        <f>SUM(C33:C37)</f>
+        <v>3.5</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
@@ -1022,16 +1040,16 @@
       <c r="C39" s="7"/>
       <c r="D39" s="9">
         <f>SUM(C33:C37)</f>
-        <v>2.5</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B41" s="15"/>
-      <c r="C41" s="15"/>
-      <c r="D41" s="15"/>
+      <c r="A41" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B41" s="16"/>
+      <c r="C41" s="16"/>
+      <c r="D41" s="16"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
@@ -1049,30 +1067,42 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
-        <v>2862</v>
-      </c>
-      <c r="B43" s="1"/>
-      <c r="C43" s="7"/>
+        <v>3221</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C43" s="7">
+        <v>1</v>
+      </c>
       <c r="D43" s="9">
         <v>9</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
-        <v>2861</v>
-      </c>
-      <c r="B44" s="1"/>
-      <c r="C44" s="7"/>
+        <v>3228</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>3</v>
+      </c>
       <c r="D44" s="9" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
-        <v>2864</v>
-      </c>
-      <c r="B45" s="1"/>
-      <c r="C45" s="7"/>
+        <v>3224</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C45" s="7">
+        <v>2</v>
+      </c>
       <c r="D45" s="9">
         <v>4</v>
       </c>
@@ -1091,7 +1121,7 @@
       <c r="C47" s="7"/>
       <c r="D47" s="10">
         <f>SUM(C43:C45)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
@@ -1108,7 +1138,7 @@
       <c r="C49" s="7"/>
       <c r="D49" s="9">
         <f>SUM(C43:C45)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new sprint planning and research doc progress
</commit_message>
<xml_diff>
--- a/Project documentation/3. Realization/Issue estimates.xlsx
+++ b/Project documentation/3. Realization/Issue estimates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rymga\Desktop\Semester 8\S8-GI-Drieam\Project documentation\3. Realization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CF040C9-BDEB-409E-88FE-06D2D0F185C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45929691-5C3A-4B8C-9F97-CE1795E81F2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1501C23A-469F-491C-9AA1-0DB21E281099}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="39">
   <si>
     <t>Description</t>
   </si>
@@ -138,6 +138,21 @@
   </si>
   <si>
     <t>Allow filtering by creation date</t>
+  </si>
+  <si>
+    <t>Add title and description in my evidence page</t>
+  </si>
+  <si>
+    <t>Add a tooltip on evidence types</t>
+  </si>
+  <si>
+    <t>Add a tooltip for goal tag status</t>
+  </si>
+  <si>
+    <t>Add status color on goal tags</t>
+  </si>
+  <si>
+    <t>Goal and collection tags need margin</t>
   </si>
 </sst>
 </file>
@@ -234,7 +249,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -274,6 +289,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Explanatory Text" xfId="2" builtinId="53"/>
@@ -590,10 +606,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{164F14AA-CFE8-4BA4-89BA-FFC874ABC001}">
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1061,9 +1077,7 @@
       <c r="C42" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D42" s="9" t="s">
-        <v>11</v>
-      </c>
+      <c r="D42" s="17"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
@@ -1075,8 +1089,8 @@
       <c r="C43" s="7">
         <v>1</v>
       </c>
-      <c r="D43" s="9">
-        <v>9</v>
+      <c r="D43" s="9" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
@@ -1086,11 +1100,11 @@
       <c r="B44" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C44" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D44" s="9" t="s">
-        <v>15</v>
+      <c r="C44" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="D44" s="9">
+        <v>9</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
@@ -1103,43 +1117,78 @@
       <c r="C45" s="7">
         <v>2</v>
       </c>
-      <c r="D45" s="9">
-        <v>4</v>
+      <c r="D45" s="9" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" s="2"/>
-      <c r="B46" s="1"/>
-      <c r="C46" s="7"/>
-      <c r="D46" s="9" t="s">
+      <c r="A46" s="2">
+        <v>3411</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C46" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="D46" s="9">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" s="2">
+        <v>3410</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C47" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="D47" s="9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47" s="2"/>
-      <c r="B47" s="1"/>
-      <c r="C47" s="7"/>
-      <c r="D47" s="10">
-        <f>SUM(C43:C45)</f>
-        <v>3</v>
-      </c>
-    </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A48" s="2"/>
-      <c r="B48" s="1"/>
-      <c r="C48" s="7"/>
-      <c r="D48" s="9" t="s">
+      <c r="A48" s="2">
+        <v>3407</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C48" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="D48" s="10">
+        <f>SUM(C43:C50)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" s="2">
+        <v>3408</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C49" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="D49" s="9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" s="2"/>
-      <c r="B49" s="1"/>
-      <c r="C49" s="7"/>
-      <c r="D49" s="9">
-        <f>SUM(C43:C45)</f>
-        <v>3</v>
-      </c>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" s="2">
+        <v>3409</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C50" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="D50" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>